<commit_message>
CN_04_08 con corrección de estilo
Solicitudes gráficas no se envían hasta saber si los recursos están o no
aprobados.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion08/EsqueletoGuion_CN_04_08_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion08/EsqueletoGuion_CN_04_08_CO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="72">
   <si>
     <t>FICHA</t>
   </si>
@@ -58,9 +58,6 @@
     <t>CLAVE</t>
   </si>
   <si>
-    <t>DESCRIPCION</t>
-  </si>
-  <si>
     <t>NIVEL</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>CN_04_08_C0</t>
   </si>
   <si>
-    <t xml:space="preserve">Todo nuestro entorno está en continuo cambio: las plantas, los animales, las cosas inanimadas, las naturales y las artificiales. Incluso uno mismo ya no es igual que hace tan solo un segundo. </t>
-  </si>
-  <si>
     <t>Educación básica primaria</t>
   </si>
   <si>
@@ -242,6 +236,12 @@
   </si>
   <si>
     <t>Competencias: identificación de los cambios de estado</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todo nuestro entorno está en continuo cambio: las plantas, los animales, las cosas inanimadas, las naturales y las artificiales. Incluso uno mismo ya no es igual a como era hace tan solo un segundo </t>
   </si>
 </sst>
 </file>
@@ -753,7 +753,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -799,6 +799,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1483,7 +1487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1496,7 +1502,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -1504,23 +1510,23 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
@@ -1533,10 +1539,10 @@
     </row>
     <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1554,7 +1560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1593,16 +1601,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>68</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1619,16 +1627,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1639,16 +1647,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -1659,16 +1667,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
         <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>68</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -1679,16 +1687,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
         <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" t="s">
-        <v>68</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -1699,16 +1707,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>68</v>
       </c>
       <c r="F7">
         <v>11</v>
@@ -1719,16 +1727,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
         <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" t="s">
-        <v>68</v>
       </c>
       <c r="F8">
         <v>15</v>
@@ -1739,16 +1747,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
         <v>66</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" t="s">
-        <v>68</v>
       </c>
       <c r="F9">
         <v>16</v>
@@ -1780,7 +1788,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,10 +1810,10 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1813,10 +1821,10 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1824,21 +1832,21 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -1846,10 +1854,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -1857,10 +1865,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -1868,10 +1876,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -1879,10 +1887,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -1890,10 +1898,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>17</v>
@@ -1901,10 +1909,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>18</v>
@@ -1912,10 +1920,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>19</v>
@@ -1923,10 +1931,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>20</v>
@@ -1934,10 +1942,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>21</v>
@@ -1991,10 +1999,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2002,10 +2010,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2013,10 +2021,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2024,10 +2032,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2035,10 +2043,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2046,10 +2054,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2057,10 +2065,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2068,10 +2076,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2079,10 +2087,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2090,10 +2098,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,10 +2109,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2112,10 +2120,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,10 +2131,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,10 +2142,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2145,10 +2153,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2156,10 +2164,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2167,10 +2175,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2178,10 +2186,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2189,10 +2197,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2200,10 +2208,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2211,10 +2219,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
@@ -2237,11 +2245,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2259,22 +2265,22 @@
         <v>6</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="H1" s="12" t="s">
         <v>3</v>
@@ -2285,13 +2291,13 @@
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -2302,13 +2308,13 @@
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>26</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -2319,13 +2325,13 @@
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2336,13 +2342,13 @@
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -2353,34 +2359,34 @@
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
@@ -2391,17 +2397,17 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
@@ -2410,17 +2416,17 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -2429,17 +2435,17 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -2448,17 +2454,17 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
@@ -2467,17 +2473,17 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="19"/>
@@ -2486,17 +2492,17 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -2505,121 +2511,124 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>36</v>
-      </c>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="5"/>
+      <c r="A18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -2629,35 +2638,33 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -2665,17 +2672,17 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -2683,117 +2690,115 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-    </row>
-    <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A26" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="17"/>
+        <v>43</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>26</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="17"/>
@@ -2801,17 +2806,17 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -2820,17 +2825,17 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
@@ -2839,131 +2844,131 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
       <c r="H31" s="17"/>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="17"/>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="17"/>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
       <c r="H34" s="17"/>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="17"/>
       <c r="I35" s="20"/>
     </row>
-    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
       <c r="H36" s="17"/>
       <c r="I36" s="20"/>
     </row>
-    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -2972,201 +2977,197 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I38" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="H38" s="17"/>
+      <c r="I38" s="20"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
-      <c r="H39" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="20"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
       <c r="H40" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="20"/>
-    </row>
-    <row r="42" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="H41" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E42" s="22" t="s">
         <v>26</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="20"/>
-    </row>
-    <row r="43" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="H42" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I42" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
       <c r="H43" s="17"/>
       <c r="I43" s="20"/>
     </row>
-    <row r="44" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F44" s="22"/>
       <c r="G44" s="22"/>
       <c r="H44" s="17"/>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F45" s="22"/>
       <c r="G45" s="22"/>
       <c r="H45" s="17"/>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
-      <c r="H46" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I46" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="H46" s="17"/>
+      <c r="I46" s="20"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E47" s="22" t="s">
         <v>25</v>
@@ -3176,133 +3177,137 @@
       <c r="H47" s="17"/>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="20"/>
-    </row>
-    <row r="49" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="H48" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I48" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
       <c r="H49" s="17"/>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="17"/>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
       <c r="H51" s="17"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
       <c r="H52" s="17"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
       <c r="H53" s="17"/>
       <c r="I53" s="20"/>
     </row>
-    <row r="54" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
@@ -3311,194 +3316,267 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
-      <c r="H55" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="I55" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="H55" s="17"/>
+      <c r="I55" s="20"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F56" s="22"/>
       <c r="G56" s="22"/>
-      <c r="H56" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I56" s="20" t="s">
-        <v>36</v>
-      </c>
+      <c r="H56" s="17"/>
+      <c r="I56" s="20"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="22" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
       <c r="H57" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I57" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="21"/>
+      <c r="D58" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I57" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="2" t="s">
+      <c r="E58" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I58" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="21"/>
+      <c r="D59" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="20"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I60" s="19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+      <c r="I61" s="9"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" t="s">
+        <v>56</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H63" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="I63" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H58" t="s">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H64" t="s">
         <v>58</v>
       </c>
-      <c r="I58" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H59" t="s">
+      <c r="I64" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" t="s">
         <v>59</v>
       </c>
-      <c r="I59" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H60" t="s">
+      <c r="I65" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H66" t="s">
         <v>60</v>
       </c>
-      <c r="I60" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>19</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H61" t="s">
+      <c r="I66" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="I61" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>19</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H62" t="s">
+      <c r="C67" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I62" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A63" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="21" t="s">
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="20" t="s">
-        <v>36</v>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección en nombres de temas esqueleto de guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion08/EsqueletoGuion_CN_04_08_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion08/EsqueletoGuion_CN_04_08_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="19440" windowHeight="11760" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="69">
   <si>
     <t>FICHA</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Átomos y moléculas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: los estados de la materia</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: composición de la materia</t>
   </si>
   <si>
@@ -194,12 +191,6 @@
   </si>
   <si>
     <t>Competencias</t>
-  </si>
-  <si>
-    <t>La materia y sus propiedades</t>
-  </si>
-  <si>
-    <t>Identifica cambios de estado</t>
   </si>
   <si>
     <t>Reconoce los puntos de fusión y ebullición</t>
@@ -1477,7 +1468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1487,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1515,10 +1506,10 @@
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1601,16 +1592,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1627,16 +1618,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1647,16 +1638,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F4">
         <v>6</v>
@@ -1667,16 +1658,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -1687,16 +1678,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -1707,16 +1698,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7">
         <v>11</v>
@@ -1727,16 +1718,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
         <v>65</v>
       </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F8">
         <v>15</v>
@@ -1747,16 +1738,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9">
         <v>16</v>
@@ -1788,7 +1779,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1834,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
@@ -1854,7 +1845,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -1865,7 +1856,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
@@ -1876,7 +1867,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -1887,7 +1878,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -1898,7 +1889,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -1909,7 +1900,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -1920,7 +1911,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
@@ -1931,7 +1922,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -1942,7 +1933,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>34</v>
@@ -2054,7 +2045,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>28</v>
@@ -2065,7 +2056,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>34</v>
@@ -2076,7 +2067,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>34</v>
@@ -2087,7 +2078,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>28</v>
@@ -2098,7 +2089,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>28</v>
@@ -2109,7 +2100,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>28</v>
@@ -2120,7 +2111,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>34</v>
@@ -2131,7 +2122,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>34</v>
@@ -2142,7 +2133,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>34</v>
@@ -2153,7 +2144,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>28</v>
@@ -2164,7 +2155,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>28</v>
@@ -2175,7 +2166,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>34</v>
@@ -2186,7 +2177,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>34</v>
@@ -2197,7 +2188,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>34</v>
@@ -2208,7 +2199,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>34</v>
@@ -2219,7 +2210,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>34</v>
@@ -2247,7 +2238,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="F47" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2723,7 +2716,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>28</v>
@@ -2764,18 +2757,18 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>42</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>43</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>23</v>
@@ -2787,12 +2780,12 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>24</v>
@@ -2809,11 +2802,11 @@
         <v>18</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>23</v>
@@ -2828,11 +2821,11 @@
         <v>18</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>24</v>
@@ -2847,11 +2840,11 @@
         <v>18</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E31" s="22" t="s">
         <v>23</v>
@@ -2866,11 +2859,11 @@
         <v>18</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E32" s="22" t="s">
         <v>24</v>
@@ -2885,11 +2878,11 @@
         <v>18</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E33" s="22" t="s">
         <v>23</v>
@@ -2904,11 +2897,11 @@
         <v>18</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="22" t="s">
         <v>23</v>
@@ -2923,11 +2916,11 @@
         <v>18</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" s="22" t="s">
         <v>24</v>
@@ -2942,11 +2935,11 @@
         <v>18</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36" s="22" t="s">
         <v>23</v>
@@ -2961,11 +2954,11 @@
         <v>18</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>24</v>
@@ -2980,11 +2973,11 @@
         <v>18</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E38" s="22" t="s">
         <v>30</v>
@@ -2999,11 +2992,11 @@
         <v>18</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E39" s="22" t="s">
         <v>24</v>
@@ -3018,11 +3011,11 @@
         <v>18</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>32</v>
@@ -3030,7 +3023,7 @@
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
       <c r="H40" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>34</v>
@@ -3041,11 +3034,11 @@
         <v>18</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E41" s="22" t="s">
         <v>32</v>
@@ -3053,7 +3046,7 @@
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
       <c r="H41" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I41" s="20" t="s">
         <v>28</v>
@@ -3064,11 +3057,11 @@
         <v>18</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E42" s="22" t="s">
         <v>26</v>
@@ -3076,7 +3069,7 @@
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
       <c r="H42" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I42" s="20" t="s">
         <v>28</v>
@@ -3087,11 +3080,11 @@
         <v>18</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E43" s="22" t="s">
         <v>23</v>
@@ -3106,11 +3099,11 @@
         <v>18</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E44" s="22" t="s">
         <v>24</v>
@@ -3125,11 +3118,11 @@
         <v>18</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E45" s="22" t="s">
         <v>23</v>
@@ -3144,11 +3137,11 @@
         <v>18</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E46" s="22" t="s">
         <v>24</v>
@@ -3163,11 +3156,11 @@
         <v>18</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E47" s="22" t="s">
         <v>25</v>
@@ -3182,11 +3175,11 @@
         <v>18</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48" s="22" t="s">
         <v>32</v>
@@ -3194,7 +3187,7 @@
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
       <c r="H48" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I48" s="20" t="s">
         <v>28</v>
@@ -3205,11 +3198,11 @@
         <v>18</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E49" s="22" t="s">
         <v>23</v>
@@ -3224,11 +3217,11 @@
         <v>18</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E50" s="22" t="s">
         <v>25</v>
@@ -3243,11 +3236,11 @@
         <v>18</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E51" s="22" t="s">
         <v>23</v>
@@ -3262,11 +3255,11 @@
         <v>18</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E52" s="22" t="s">
         <v>24</v>
@@ -3281,11 +3274,11 @@
         <v>18</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53" s="22" t="s">
         <v>23</v>
@@ -3300,11 +3293,11 @@
         <v>18</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E54" s="22" t="s">
         <v>24</v>
@@ -3319,11 +3312,11 @@
         <v>18</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C55" s="21"/>
       <c r="D55" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E55" s="22" t="s">
         <v>23</v>
@@ -3338,11 +3331,11 @@
         <v>18</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C56" s="21"/>
       <c r="D56" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E56" s="22" t="s">
         <v>25</v>
@@ -3357,11 +3350,11 @@
         <v>18</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E57" s="22" t="s">
         <v>26</v>
@@ -3369,7 +3362,7 @@
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
       <c r="H57" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I57" s="20" t="s">
         <v>34</v>
@@ -3380,11 +3373,11 @@
         <v>18</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E58" s="22" t="s">
         <v>26</v>
@@ -3392,7 +3385,7 @@
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
       <c r="H58" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I58" s="20" t="s">
         <v>34</v>
@@ -3403,7 +3396,7 @@
         <v>18</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="22" t="s">
@@ -3422,7 +3415,7 @@
         <v>18</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C60" s="21"/>
       <c r="D60" s="22" t="s">
@@ -3434,7 +3427,7 @@
       <c r="F60" s="22"/>
       <c r="G60" s="22"/>
       <c r="H60" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I60" s="19" t="s">
         <v>34</v>
@@ -3445,7 +3438,7 @@
         <v>18</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" s="23" t="s">
         <v>23</v>
@@ -3461,13 +3454,13 @@
         <v>18</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H62" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>28</v>
@@ -3478,13 +3471,13 @@
         <v>18</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H63" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>28</v>
@@ -3495,13 +3488,13 @@
         <v>18</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H64" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I64" s="5" t="s">
         <v>34</v>
@@ -3512,13 +3505,13 @@
         <v>18</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H65" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>34</v>
@@ -3529,13 +3522,13 @@
         <v>18</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>34</v>
@@ -3546,10 +3539,10 @@
         <v>18</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D67" s="22"/>
       <c r="E67" s="22"/>
@@ -3565,10 +3558,10 @@
         <v>18</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>

</xml_diff>